<commit_message>
Remove test variable reassignment that isn't one of the variables we want to reassign to a new topic.
</commit_message>
<xml_diff>
--- a/Topics_to_be_changed.xlsx
+++ b/Topics_to_be_changed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\o.lyttleton\Development\colectica-api\issue-51\colectica-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B3A331-0754-4F75-B56A-4A17AF5DAC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD96202-F2A8-4AE0-998B-B08A06755ABB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="380" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="496">
   <si>
     <t>Variable Label</t>
   </si>
@@ -1525,12 +1525,6 @@
   </si>
   <si>
     <t>H109/H96: Stereo: Type of headphones used normally: hearing: F11</t>
-  </si>
-  <si>
-    <t>ca_hstime_mnspid</t>
-  </si>
-  <si>
-    <t>Time taken</t>
   </si>
 </sst>
 </file>
@@ -1890,10 +1884,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E364"/>
+  <dimension ref="A1:E363"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A346" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1922,20 +1916,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>496</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>497</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1">
         <v>11607</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>11608</v>
       </c>
     </row>
@@ -1944,7 +1938,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
@@ -1961,7 +1955,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
@@ -1974,11 +1968,11 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
+      <c r="A5" s="6" t="s">
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -1995,7 +1989,7 @@
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -2012,7 +2006,7 @@
         <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
@@ -2029,7 +2023,7 @@
         <v>42</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
@@ -2046,7 +2040,7 @@
         <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
@@ -2063,7 +2057,7 @@
         <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
@@ -2080,7 +2074,7 @@
         <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -2097,7 +2091,7 @@
         <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>17</v>
@@ -2114,7 +2108,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
         <v>17</v>
@@ -2131,7 +2125,7 @@
         <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>17</v>
@@ -2144,11 +2138,11 @@
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>42</v>
+      <c r="A15" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -2165,7 +2159,7 @@
         <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
@@ -2182,7 +2176,7 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -2199,7 +2193,7 @@
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
@@ -2216,7 +2210,7 @@
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>
@@ -2233,7 +2227,7 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
@@ -2250,7 +2244,7 @@
         <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
@@ -2267,7 +2261,7 @@
         <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
         <v>17</v>
@@ -2280,20 +2274,20 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="1">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="3">
         <v>11607</v>
       </c>
       <c r="E23" s="3">
-        <v>11608</v>
+        <v>11609</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2301,10 +2295,10 @@
         <v>42</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D24" s="3">
         <v>11607</v>
@@ -2318,10 +2312,10 @@
         <v>42</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D25" s="3">
         <v>11607</v>
@@ -2335,10 +2329,10 @@
         <v>42</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D26" s="3">
         <v>11607</v>
@@ -2352,10 +2346,10 @@
         <v>42</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D27" s="3">
         <v>11607</v>
@@ -2369,10 +2363,10 @@
         <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D28" s="3">
         <v>11607</v>
@@ -2386,10 +2380,10 @@
         <v>42</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D29" s="3">
         <v>11607</v>
@@ -2403,10 +2397,10 @@
         <v>42</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D30" s="3">
         <v>11607</v>
@@ -2420,10 +2414,10 @@
         <v>42</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>146</v>
+        <v>44</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="D31" s="3">
         <v>11607</v>
@@ -2437,10 +2431,10 @@
         <v>42</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D32" s="3">
         <v>11607</v>
@@ -2454,10 +2448,10 @@
         <v>42</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D33" s="3">
         <v>11607</v>
@@ -2471,10 +2465,10 @@
         <v>42</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D34" s="3">
         <v>11607</v>
@@ -2488,10 +2482,10 @@
         <v>42</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D35" s="3">
         <v>11607</v>
@@ -2505,10 +2499,10 @@
         <v>42</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D36" s="3">
         <v>11607</v>
@@ -2522,10 +2516,10 @@
         <v>42</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D37" s="3">
         <v>11607</v>
@@ -2535,37 +2529,37 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>42</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="3">
-        <v>11607</v>
+      <c r="A38" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38" t="s">
+        <v>91</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="1">
+        <v>116</v>
       </c>
       <c r="E38" s="3">
-        <v>11609</v>
+        <v>11603</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B39" t="s">
-        <v>91</v>
+      <c r="B39" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="C39" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="D39" s="1">
         <v>116</v>
       </c>
       <c r="E39" s="3">
-        <v>11603</v>
+        <v>11605</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2573,84 +2567,84 @@
         <v>50</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="C40" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D40" s="1">
         <v>116</v>
       </c>
       <c r="E40" s="3">
-        <v>11605</v>
+        <v>11610</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1" t="s">
+      <c r="A41" t="s">
         <v>50</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C41" t="s">
-        <v>68</v>
-      </c>
-      <c r="D41" s="1">
+      <c r="B41" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="3">
+        <v>11602</v>
+      </c>
+      <c r="E41" s="3">
+        <v>11607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D42" s="1">
         <v>116</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E42" s="3">
         <v>11610</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D42" s="3">
-        <v>11602</v>
-      </c>
-      <c r="E42" s="3">
-        <v>11607</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>70</v>
+      <c r="B43" t="s">
+        <v>98</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
-      </c>
-      <c r="D43" s="1">
-        <v>116</v>
+        <v>99</v>
+      </c>
+      <c r="D43">
+        <v>11615</v>
       </c>
       <c r="E43" s="3">
-        <v>11610</v>
+        <v>11604</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="1" t="s">
+      <c r="A44" t="s">
         <v>50</v>
       </c>
-      <c r="B44" t="s">
-        <v>98</v>
-      </c>
-      <c r="C44" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44">
-        <v>11615</v>
+      <c r="B44" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="3">
+        <v>11607</v>
       </c>
       <c r="E44" s="3">
-        <v>11604</v>
+        <v>11609</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2658,10 +2652,10 @@
         <v>50</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>109</v>
+        <v>133</v>
       </c>
       <c r="D45" s="3">
         <v>11607</v>
@@ -2675,10 +2669,10 @@
         <v>50</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D46" s="3">
         <v>11607</v>
@@ -2692,10 +2686,10 @@
         <v>50</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D47" s="3">
         <v>11607</v>
@@ -2709,10 +2703,10 @@
         <v>50</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D48" s="3">
         <v>11607</v>
@@ -2726,10 +2720,10 @@
         <v>50</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D49" s="3">
         <v>11607</v>
@@ -2743,10 +2737,10 @@
         <v>50</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D50" s="3">
         <v>11607</v>
@@ -2760,10 +2754,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D51" s="3">
         <v>11607</v>
@@ -2777,10 +2771,10 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>153</v>
+        <v>51</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="D52" s="3">
         <v>11607</v>
@@ -2794,10 +2788,10 @@
         <v>50</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D53" s="3">
         <v>11607</v>
@@ -2811,10 +2805,10 @@
         <v>50</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D54" s="3">
         <v>11607</v>
@@ -2828,10 +2822,10 @@
         <v>50</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D55" s="3">
         <v>11607</v>
@@ -2845,10 +2839,10 @@
         <v>50</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D56" s="3">
         <v>11607</v>
@@ -2862,10 +2856,10 @@
         <v>50</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D57" s="3">
         <v>11607</v>
@@ -2879,10 +2873,10 @@
         <v>50</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D58" s="3">
         <v>11607</v>
@@ -2891,32 +2885,32 @@
         <v>11609</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D59" s="3">
-        <v>11607</v>
+    <row r="59" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" t="s">
+        <v>68</v>
+      </c>
+      <c r="D59" s="1">
+        <v>11603</v>
       </c>
       <c r="E59" s="3">
-        <v>11609</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+        <v>11610</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C60" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D60" s="1">
         <v>11603</v>
@@ -2925,69 +2919,69 @@
         <v>11610</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C61" t="s">
-        <v>71</v>
-      </c>
-      <c r="D61" s="1">
-        <v>11603</v>
+    <row r="61" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>114</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D61" s="3">
+        <v>11605</v>
       </c>
       <c r="E61" s="3">
         <v>11610</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>114</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="D62" s="3">
-        <v>11605</v>
+        <v>11607</v>
       </c>
       <c r="E62" s="3">
-        <v>11610</v>
+        <v>11602</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>114</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D63" s="3">
+        <v>80</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D63">
         <v>11607</v>
       </c>
       <c r="E63" s="3">
-        <v>11602</v>
+        <v>11603</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>80</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>94</v>
+      <c r="B64" t="s">
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
-      </c>
-      <c r="D64">
-        <v>11607</v>
+        <v>89</v>
+      </c>
+      <c r="D64" s="1">
+        <v>116</v>
       </c>
       <c r="E64" s="3">
         <v>11603</v>
@@ -2998,7 +2992,7 @@
         <v>80</v>
       </c>
       <c r="B65" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
         <v>89</v>
@@ -3015,7 +3009,7 @@
         <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
         <v>89</v>
@@ -3032,7 +3026,7 @@
         <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C67" t="s">
         <v>89</v>
@@ -3049,7 +3043,7 @@
         <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
         <v>89</v>
@@ -3066,7 +3060,7 @@
         <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C69" t="s">
         <v>89</v>
@@ -3083,7 +3077,7 @@
         <v>80</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C70" t="s">
         <v>89</v>
@@ -3097,13 +3091,13 @@
     </row>
     <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B71" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C71" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D71" s="1">
         <v>116</v>
@@ -3116,17 +3110,17 @@
       <c r="A72" t="s">
         <v>73</v>
       </c>
-      <c r="B72" t="s">
-        <v>88</v>
+      <c r="B72" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>90</v>
-      </c>
-      <c r="D72" s="1">
-        <v>116</v>
+        <v>78</v>
+      </c>
+      <c r="D72">
+        <v>11604</v>
       </c>
       <c r="E72" s="3">
-        <v>11603</v>
+        <v>11610</v>
       </c>
     </row>
     <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -3134,10 +3128,10 @@
         <v>73</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D73">
         <v>11604</v>
@@ -3151,10 +3145,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C74" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D74">
         <v>11604</v>
@@ -3167,39 +3161,39 @@
       <c r="A75" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>75</v>
+      <c r="B75" t="s">
+        <v>116</v>
       </c>
       <c r="C75" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="D75">
         <v>11604</v>
       </c>
       <c r="E75" s="3">
-        <v>11610</v>
+        <v>11607</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>73</v>
-      </c>
-      <c r="B76" t="s">
-        <v>116</v>
+        <v>38</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C76" t="s">
-        <v>117</v>
-      </c>
-      <c r="D76">
-        <v>11604</v>
+        <v>14</v>
+      </c>
+      <c r="D76" s="1">
+        <v>11607</v>
       </c>
       <c r="E76" s="3">
-        <v>11607</v>
+        <v>11601</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>3</v>
@@ -3216,7 +3210,7 @@
     </row>
     <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>3</v>
@@ -3233,7 +3227,7 @@
     </row>
     <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>3</v>
@@ -3250,7 +3244,7 @@
     </row>
     <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>3</v>
@@ -3267,10 +3261,10 @@
     </row>
     <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C81" t="s">
         <v>14</v>
@@ -3284,7 +3278,7 @@
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>4</v>
@@ -3301,7 +3295,7 @@
     </row>
     <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>4</v>
@@ -3318,7 +3312,7 @@
     </row>
     <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>4</v>
@@ -3335,7 +3329,7 @@
     </row>
     <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>4</v>
@@ -3352,10 +3346,10 @@
     </row>
     <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C86" t="s">
         <v>14</v>
@@ -3369,7 +3363,7 @@
     </row>
     <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>5</v>
@@ -3386,7 +3380,7 @@
     </row>
     <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>5</v>
@@ -3403,7 +3397,7 @@
     </row>
     <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
@@ -3420,7 +3414,7 @@
     </row>
     <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>5</v>
@@ -3437,10 +3431,10 @@
     </row>
     <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C91" t="s">
         <v>14</v>
@@ -3454,7 +3448,7 @@
     </row>
     <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>6</v>
@@ -3471,7 +3465,7 @@
     </row>
     <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>6</v>
@@ -3488,7 +3482,7 @@
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>6</v>
@@ -3505,7 +3499,7 @@
     </row>
     <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>6</v>
@@ -3522,10 +3516,10 @@
     </row>
     <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C96" t="s">
         <v>14</v>
@@ -3539,7 +3533,7 @@
     </row>
     <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>7</v>
@@ -3556,7 +3550,7 @@
     </row>
     <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>7</v>
@@ -3573,7 +3567,7 @@
     </row>
     <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>7</v>
@@ -3590,7 +3584,7 @@
     </row>
     <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>7</v>
@@ -3607,10 +3601,10 @@
     </row>
     <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C101" t="s">
         <v>14</v>
@@ -3624,7 +3618,7 @@
     </row>
     <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>8</v>
@@ -3641,7 +3635,7 @@
     </row>
     <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>8</v>
@@ -3656,9 +3650,9 @@
         <v>11601</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>8</v>
@@ -3675,7 +3669,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>8</v>
@@ -3692,10 +3686,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C106" t="s">
         <v>14</v>
@@ -3709,7 +3703,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>9</v>
@@ -3726,7 +3720,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>9</v>
@@ -3743,7 +3737,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>9</v>
@@ -3760,7 +3754,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>9</v>
@@ -3777,10 +3771,10 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C111" t="s">
         <v>14</v>
@@ -3794,7 +3788,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>10</v>
@@ -3811,7 +3805,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>10</v>
@@ -3826,9 +3820,9 @@
         <v>11601</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>10</v>
@@ -3845,7 +3839,7 @@
     </row>
     <row r="115" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>10</v>
@@ -3862,10 +3856,10 @@
     </row>
     <row r="116" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C116" t="s">
         <v>14</v>
@@ -3879,7 +3873,7 @@
     </row>
     <row r="117" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>11</v>
@@ -3896,7 +3890,7 @@
     </row>
     <row r="118" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>11</v>
@@ -3913,7 +3907,7 @@
     </row>
     <row r="119" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>11</v>
@@ -3930,7 +3924,7 @@
     </row>
     <row r="120" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>11</v>
@@ -3947,10 +3941,10 @@
     </row>
     <row r="121" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C121" t="s">
         <v>14</v>
@@ -3964,7 +3958,7 @@
     </row>
     <row r="122" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>12</v>
@@ -3981,7 +3975,7 @@
     </row>
     <row r="123" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>12</v>
@@ -3998,7 +3992,7 @@
     </row>
     <row r="124" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>12</v>
@@ -4015,7 +4009,7 @@
     </row>
     <row r="125" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>12</v>
@@ -4032,24 +4026,24 @@
     </row>
     <row r="126" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C126" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
       <c r="D126" s="1">
-        <v>11607</v>
+        <v>11603</v>
       </c>
       <c r="E126" s="3">
-        <v>11601</v>
+        <v>11605</v>
       </c>
     </row>
     <row r="127" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>60</v>
@@ -4064,9 +4058,9 @@
         <v>11605</v>
       </c>
     </row>
-    <row r="128" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>60</v>
@@ -4083,7 +4077,7 @@
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>60</v>
@@ -4100,7 +4094,7 @@
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>60</v>
@@ -4115,12 +4109,12 @@
         <v>11605</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C131" t="s">
         <v>66</v>
@@ -4134,7 +4128,7 @@
     </row>
     <row r="132" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>61</v>
@@ -4151,7 +4145,7 @@
     </row>
     <row r="133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>61</v>
@@ -4168,7 +4162,7 @@
     </row>
     <row r="134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>61</v>
@@ -4185,7 +4179,7 @@
     </row>
     <row r="135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>61</v>
@@ -4202,10 +4196,10 @@
     </row>
     <row r="136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C136" t="s">
         <v>66</v>
@@ -4219,7 +4213,7 @@
     </row>
     <row r="137" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>62</v>
@@ -4236,7 +4230,7 @@
     </row>
     <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>62</v>
@@ -4253,7 +4247,7 @@
     </row>
     <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>62</v>
@@ -4270,7 +4264,7 @@
     </row>
     <row r="140" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>62</v>
@@ -4287,10 +4281,10 @@
     </row>
     <row r="141" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C141" t="s">
         <v>66</v>
@@ -4304,7 +4298,7 @@
     </row>
     <row r="142" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>63</v>
@@ -4321,7 +4315,7 @@
     </row>
     <row r="143" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>63</v>
@@ -4338,7 +4332,7 @@
     </row>
     <row r="144" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>63</v>
@@ -4355,7 +4349,7 @@
     </row>
     <row r="145" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>63</v>
@@ -4372,10 +4366,10 @@
     </row>
     <row r="146" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C146" t="s">
         <v>66</v>
@@ -4389,7 +4383,7 @@
     </row>
     <row r="147" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>64</v>
@@ -4406,7 +4400,7 @@
     </row>
     <row r="148" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>64</v>
@@ -4423,7 +4417,7 @@
     </row>
     <row r="149" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>64</v>
@@ -4440,7 +4434,7 @@
     </row>
     <row r="150" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>64</v>
@@ -4457,10 +4451,10 @@
     </row>
     <row r="151" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C151" t="s">
         <v>66</v>
@@ -4474,7 +4468,7 @@
     </row>
     <row r="152" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>65</v>
@@ -4491,7 +4485,7 @@
     </row>
     <row r="153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>65</v>
@@ -4508,7 +4502,7 @@
     </row>
     <row r="154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>65</v>
@@ -4525,7 +4519,7 @@
     </row>
     <row r="155" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>65</v>
@@ -4542,41 +4536,41 @@
     </row>
     <row r="156" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>37</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>65</v>
+        <v>126</v>
+      </c>
+      <c r="B156" t="s">
+        <v>127</v>
       </c>
       <c r="C156" t="s">
-        <v>66</v>
-      </c>
-      <c r="D156" s="1">
-        <v>11603</v>
+        <v>128</v>
+      </c>
+      <c r="D156">
+        <v>11615</v>
       </c>
       <c r="E156" s="3">
-        <v>11605</v>
+        <v>11601</v>
       </c>
     </row>
     <row r="157" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B157" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C157" t="s">
-        <v>128</v>
-      </c>
-      <c r="D157">
-        <v>11615</v>
+        <v>66</v>
+      </c>
+      <c r="D157" s="1">
+        <v>11603</v>
       </c>
       <c r="E157" s="3">
-        <v>11601</v>
+        <v>11605</v>
       </c>
     </row>
     <row r="158" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B158" t="s">
         <v>119</v>
@@ -4593,7 +4587,7 @@
     </row>
     <row r="159" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B159" t="s">
         <v>119</v>
@@ -4610,7 +4604,7 @@
     </row>
     <row r="160" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B160" t="s">
         <v>119</v>
@@ -4627,7 +4621,7 @@
     </row>
     <row r="161" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B161" t="s">
         <v>119</v>
@@ -4644,10 +4638,10 @@
     </row>
     <row r="162" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B162" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C162" t="s">
         <v>66</v>
@@ -4661,7 +4655,7 @@
     </row>
     <row r="163" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B163" t="s">
         <v>120</v>
@@ -4678,7 +4672,7 @@
     </row>
     <row r="164" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B164" t="s">
         <v>120</v>
@@ -4695,7 +4689,7 @@
     </row>
     <row r="165" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B165" t="s">
         <v>120</v>
@@ -4712,7 +4706,7 @@
     </row>
     <row r="166" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B166" t="s">
         <v>120</v>
@@ -4729,10 +4723,10 @@
     </row>
     <row r="167" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B167" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C167" t="s">
         <v>66</v>
@@ -4746,7 +4740,7 @@
     </row>
     <row r="168" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B168" t="s">
         <v>121</v>
@@ -4763,7 +4757,7 @@
     </row>
     <row r="169" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B169" t="s">
         <v>121</v>
@@ -4780,7 +4774,7 @@
     </row>
     <row r="170" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B170" t="s">
         <v>121</v>
@@ -4797,7 +4791,7 @@
     </row>
     <row r="171" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B171" t="s">
         <v>121</v>
@@ -4814,10 +4808,10 @@
     </row>
     <row r="172" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B172" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C172" t="s">
         <v>66</v>
@@ -4831,7 +4825,7 @@
     </row>
     <row r="173" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B173" t="s">
         <v>122</v>
@@ -4848,7 +4842,7 @@
     </row>
     <row r="174" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B174" t="s">
         <v>122</v>
@@ -4865,7 +4859,7 @@
     </row>
     <row r="175" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B175" t="s">
         <v>122</v>
@@ -4882,7 +4876,7 @@
     </row>
     <row r="176" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B176" t="s">
         <v>122</v>
@@ -4899,10 +4893,10 @@
     </row>
     <row r="177" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B177" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C177" t="s">
         <v>66</v>
@@ -4916,7 +4910,7 @@
     </row>
     <row r="178" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B178" t="s">
         <v>123</v>
@@ -4933,7 +4927,7 @@
     </row>
     <row r="179" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B179" t="s">
         <v>123</v>
@@ -4950,7 +4944,7 @@
     </row>
     <row r="180" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B180" t="s">
         <v>123</v>
@@ -4967,7 +4961,7 @@
     </row>
     <row r="181" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B181" t="s">
         <v>123</v>
@@ -4984,10 +4978,10 @@
     </row>
     <row r="182" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B182" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C182" t="s">
         <v>66</v>
@@ -5001,7 +4995,7 @@
     </row>
     <row r="183" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B183" t="s">
         <v>124</v>
@@ -5018,7 +5012,7 @@
     </row>
     <row r="184" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B184" t="s">
         <v>124</v>
@@ -5035,7 +5029,7 @@
     </row>
     <row r="185" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B185" t="s">
         <v>124</v>
@@ -5052,7 +5046,7 @@
     </row>
     <row r="186" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B186" t="s">
         <v>124</v>
@@ -5069,24 +5063,24 @@
     </row>
     <row r="187" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B187" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="C187" t="s">
-        <v>66</v>
-      </c>
-      <c r="D187" s="1">
-        <v>11603</v>
+        <v>155</v>
+      </c>
+      <c r="D187">
+        <v>11602</v>
       </c>
       <c r="E187" s="3">
-        <v>11605</v>
+        <v>11601</v>
       </c>
     </row>
     <row r="188" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B188" t="s">
         <v>154</v>
@@ -5103,7 +5097,7 @@
     </row>
     <row r="189" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B189" t="s">
         <v>154</v>
@@ -5120,7 +5114,7 @@
     </row>
     <row r="190" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B190" t="s">
         <v>154</v>
@@ -5137,7 +5131,7 @@
     </row>
     <row r="191" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B191" t="s">
         <v>154</v>
@@ -5154,19 +5148,19 @@
     </row>
     <row r="192" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="B192" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C192" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="D192">
-        <v>11602</v>
+        <v>10810</v>
       </c>
       <c r="E192" s="3">
-        <v>11601</v>
+        <v>115</v>
       </c>
     </row>
     <row r="193" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5174,10 +5168,10 @@
         <v>157</v>
       </c>
       <c r="B193" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C193" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D193">
         <v>10810</v>
@@ -5191,10 +5185,10 @@
         <v>157</v>
       </c>
       <c r="B194" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C194" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D194">
         <v>10810</v>
@@ -5208,10 +5202,10 @@
         <v>157</v>
       </c>
       <c r="B195" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C195" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D195">
         <v>10810</v>
@@ -5225,16 +5219,16 @@
         <v>157</v>
       </c>
       <c r="B196" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
       <c r="C196" t="s">
-        <v>167</v>
+        <v>207</v>
       </c>
       <c r="D196">
-        <v>10810</v>
+        <v>115</v>
       </c>
       <c r="E196" s="3">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="197" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -5242,10 +5236,10 @@
         <v>157</v>
       </c>
       <c r="B197" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C197" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D197">
         <v>115</v>
@@ -5259,10 +5253,10 @@
         <v>157</v>
       </c>
       <c r="B198" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C198" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D198">
         <v>115</v>
@@ -5271,15 +5265,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>157</v>
       </c>
       <c r="B199" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C199" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D199">
         <v>115</v>
@@ -5293,10 +5287,10 @@
         <v>157</v>
       </c>
       <c r="B200" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C200" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D200">
         <v>115</v>
@@ -5310,10 +5304,10 @@
         <v>157</v>
       </c>
       <c r="B201" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C201" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D201">
         <v>115</v>
@@ -5327,10 +5321,10 @@
         <v>157</v>
       </c>
       <c r="B202" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C202" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D202">
         <v>115</v>
@@ -5344,10 +5338,10 @@
         <v>157</v>
       </c>
       <c r="B203" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C203" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D203">
         <v>115</v>
@@ -5361,16 +5355,16 @@
         <v>157</v>
       </c>
       <c r="B204" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="C204" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="D204">
         <v>115</v>
       </c>
       <c r="E204" s="3">
-        <v>104</v>
+        <v>107</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.35">
@@ -5378,10 +5372,10 @@
         <v>157</v>
       </c>
       <c r="B205" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C205" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D205">
         <v>115</v>
@@ -5395,10 +5389,10 @@
         <v>157</v>
       </c>
       <c r="B206" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C206" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D206">
         <v>115</v>
@@ -5412,10 +5406,10 @@
         <v>157</v>
       </c>
       <c r="B207" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C207" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D207">
         <v>115</v>
@@ -5429,10 +5423,10 @@
         <v>157</v>
       </c>
       <c r="B208" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C208" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D208">
         <v>115</v>
@@ -5446,10 +5440,10 @@
         <v>157</v>
       </c>
       <c r="B209" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C209" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D209">
         <v>115</v>
@@ -5463,16 +5457,16 @@
         <v>157</v>
       </c>
       <c r="B210" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
       <c r="C210" t="s">
-        <v>199</v>
+        <v>225</v>
       </c>
       <c r="D210">
-        <v>115</v>
+        <v>10308</v>
       </c>
       <c r="E210" s="3">
-        <v>107</v>
+        <v>10309</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.35">
@@ -5480,10 +5474,10 @@
         <v>157</v>
       </c>
       <c r="B211" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C211" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D211">
         <v>10308</v>
@@ -5497,10 +5491,10 @@
         <v>157</v>
       </c>
       <c r="B212" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C212" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D212">
         <v>10308</v>
@@ -5514,10 +5508,10 @@
         <v>157</v>
       </c>
       <c r="B213" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C213" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D213">
         <v>10308</v>
@@ -5531,10 +5525,10 @@
         <v>157</v>
       </c>
       <c r="B214" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="C214" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D214">
         <v>10308</v>
@@ -5548,10 +5542,10 @@
         <v>157</v>
       </c>
       <c r="B215" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C215" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D215">
         <v>10308</v>
@@ -5565,10 +5559,10 @@
         <v>157</v>
       </c>
       <c r="B216" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C216" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D216">
         <v>10308</v>
@@ -5582,10 +5576,10 @@
         <v>157</v>
       </c>
       <c r="B217" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C217" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D217">
         <v>10308</v>
@@ -5599,10 +5593,10 @@
         <v>157</v>
       </c>
       <c r="B218" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C218" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D218">
         <v>10308</v>
@@ -5616,10 +5610,10 @@
         <v>157</v>
       </c>
       <c r="B219" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="C219" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D219">
         <v>10308</v>
@@ -5633,10 +5627,10 @@
         <v>157</v>
       </c>
       <c r="B220" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C220" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D220">
         <v>10308</v>
@@ -5650,10 +5644,10 @@
         <v>157</v>
       </c>
       <c r="B221" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="C221" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D221">
         <v>10308</v>
@@ -5667,10 +5661,10 @@
         <v>157</v>
       </c>
       <c r="B222" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="C222" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D222">
         <v>10308</v>
@@ -5684,10 +5678,10 @@
         <v>157</v>
       </c>
       <c r="B223" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C223" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D223">
         <v>10308</v>
@@ -5701,10 +5695,10 @@
         <v>157</v>
       </c>
       <c r="B224" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C224" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D224">
         <v>10308</v>
@@ -5718,10 +5712,10 @@
         <v>157</v>
       </c>
       <c r="B225" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C225" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D225">
         <v>10308</v>
@@ -5735,10 +5729,10 @@
         <v>157</v>
       </c>
       <c r="B226" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C226" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D226">
         <v>10308</v>
@@ -5747,15 +5741,15 @@
         <v>10309</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>157</v>
       </c>
       <c r="B227" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="C227" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D227">
         <v>10308</v>
@@ -5764,15 +5758,15 @@
         <v>10309</v>
       </c>
     </row>
-    <row r="228" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>157</v>
       </c>
       <c r="B228" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C228" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D228">
         <v>10308</v>
@@ -5786,10 +5780,10 @@
         <v>157</v>
       </c>
       <c r="B229" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C229" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D229">
         <v>10308</v>
@@ -5803,10 +5797,10 @@
         <v>157</v>
       </c>
       <c r="B230" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C230" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D230">
         <v>10308</v>
@@ -5820,10 +5814,10 @@
         <v>157</v>
       </c>
       <c r="B231" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C231" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D231">
         <v>10308</v>
@@ -5837,10 +5831,10 @@
         <v>157</v>
       </c>
       <c r="B232" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="C232" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D232">
         <v>10308</v>
@@ -5854,10 +5848,10 @@
         <v>157</v>
       </c>
       <c r="B233" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C233" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D233">
         <v>10308</v>
@@ -5871,10 +5865,10 @@
         <v>157</v>
       </c>
       <c r="B234" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C234" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D234">
         <v>10308</v>
@@ -5888,10 +5882,10 @@
         <v>157</v>
       </c>
       <c r="B235" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C235" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D235">
         <v>10308</v>
@@ -5905,10 +5899,10 @@
         <v>157</v>
       </c>
       <c r="B236" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C236" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D236">
         <v>10308</v>
@@ -5922,10 +5916,10 @@
         <v>157</v>
       </c>
       <c r="B237" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C237" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D237">
         <v>10308</v>
@@ -5939,10 +5933,10 @@
         <v>157</v>
       </c>
       <c r="B238" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C238" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D238">
         <v>10308</v>
@@ -5956,10 +5950,10 @@
         <v>157</v>
       </c>
       <c r="B239" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C239" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D239">
         <v>10308</v>
@@ -5973,10 +5967,10 @@
         <v>157</v>
       </c>
       <c r="B240" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C240" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D240">
         <v>10308</v>
@@ -5990,10 +5984,10 @@
         <v>157</v>
       </c>
       <c r="B241" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C241" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D241">
         <v>10308</v>
@@ -6007,10 +6001,10 @@
         <v>157</v>
       </c>
       <c r="B242" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C242" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D242">
         <v>10308</v>
@@ -6024,10 +6018,10 @@
         <v>157</v>
       </c>
       <c r="B243" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C243" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D243">
         <v>10308</v>
@@ -6041,10 +6035,10 @@
         <v>157</v>
       </c>
       <c r="B244" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C244" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D244">
         <v>10308</v>
@@ -6058,10 +6052,10 @@
         <v>157</v>
       </c>
       <c r="B245" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C245" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D245">
         <v>10308</v>
@@ -6075,10 +6069,10 @@
         <v>157</v>
       </c>
       <c r="B246" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C246" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D246">
         <v>10308</v>
@@ -6092,10 +6086,10 @@
         <v>157</v>
       </c>
       <c r="B247" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C247" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D247">
         <v>10308</v>
@@ -6109,10 +6103,10 @@
         <v>157</v>
       </c>
       <c r="B248" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C248" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D248">
         <v>10308</v>
@@ -6126,10 +6120,10 @@
         <v>157</v>
       </c>
       <c r="B249" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C249" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D249">
         <v>10308</v>
@@ -6143,10 +6137,10 @@
         <v>157</v>
       </c>
       <c r="B250" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C250" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D250">
         <v>10308</v>
@@ -6160,10 +6154,10 @@
         <v>157</v>
       </c>
       <c r="B251" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C251" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D251">
         <v>10308</v>
@@ -6177,10 +6171,10 @@
         <v>157</v>
       </c>
       <c r="B252" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C252" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D252">
         <v>10308</v>
@@ -6194,10 +6188,10 @@
         <v>157</v>
       </c>
       <c r="B253" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C253" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D253">
         <v>10308</v>
@@ -6211,10 +6205,10 @@
         <v>157</v>
       </c>
       <c r="B254" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C254" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D254">
         <v>10308</v>
@@ -6228,10 +6222,10 @@
         <v>157</v>
       </c>
       <c r="B255" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C255" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D255">
         <v>10308</v>
@@ -6245,10 +6239,10 @@
         <v>157</v>
       </c>
       <c r="B256" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C256" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D256">
         <v>10308</v>
@@ -6262,10 +6256,10 @@
         <v>157</v>
       </c>
       <c r="B257" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C257" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D257">
         <v>10308</v>
@@ -6279,10 +6273,10 @@
         <v>157</v>
       </c>
       <c r="B258" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C258" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D258">
         <v>10308</v>
@@ -6296,10 +6290,10 @@
         <v>157</v>
       </c>
       <c r="B259" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="C259" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D259">
         <v>10308</v>
@@ -6308,15 +6302,15 @@
         <v>10309</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
         <v>157</v>
       </c>
       <c r="B260" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C260" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D260">
         <v>10308</v>
@@ -6325,15 +6319,15 @@
         <v>10309</v>
       </c>
     </row>
-    <row r="261" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>157</v>
       </c>
       <c r="B261" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C261" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D261">
         <v>10308</v>
@@ -6347,10 +6341,10 @@
         <v>157</v>
       </c>
       <c r="B262" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C262" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D262">
         <v>10308</v>
@@ -6359,15 +6353,15 @@
         <v>10309</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>157</v>
       </c>
       <c r="B263" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C263" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D263">
         <v>10308</v>
@@ -6376,15 +6370,15 @@
         <v>10309</v>
       </c>
     </row>
-    <row r="264" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>157</v>
       </c>
       <c r="B264" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C264" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D264">
         <v>10308</v>
@@ -6398,10 +6392,10 @@
         <v>157</v>
       </c>
       <c r="B265" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C265" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D265">
         <v>10308</v>
@@ -6415,10 +6409,10 @@
         <v>157</v>
       </c>
       <c r="B266" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C266" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D266">
         <v>10308</v>
@@ -6432,10 +6426,10 @@
         <v>157</v>
       </c>
       <c r="B267" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C267" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D267">
         <v>10308</v>
@@ -6449,10 +6443,10 @@
         <v>157</v>
       </c>
       <c r="B268" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="C268" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D268">
         <v>10308</v>
@@ -6466,10 +6460,10 @@
         <v>157</v>
       </c>
       <c r="B269" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C269" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D269">
         <v>10308</v>
@@ -6483,10 +6477,10 @@
         <v>157</v>
       </c>
       <c r="B270" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C270" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D270">
         <v>10308</v>
@@ -6500,10 +6494,10 @@
         <v>157</v>
       </c>
       <c r="B271" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="C271" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D271">
         <v>10308</v>
@@ -6517,10 +6511,10 @@
         <v>157</v>
       </c>
       <c r="B272" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C272" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D272">
         <v>10308</v>
@@ -6534,10 +6528,10 @@
         <v>157</v>
       </c>
       <c r="B273" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C273" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D273">
         <v>10308</v>
@@ -6551,10 +6545,10 @@
         <v>157</v>
       </c>
       <c r="B274" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C274" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D274">
         <v>10308</v>
@@ -6568,10 +6562,10 @@
         <v>157</v>
       </c>
       <c r="B275" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="C275" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D275">
         <v>10308</v>
@@ -6585,10 +6579,10 @@
         <v>157</v>
       </c>
       <c r="B276" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C276" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D276">
         <v>10308</v>
@@ -6602,10 +6596,10 @@
         <v>157</v>
       </c>
       <c r="B277" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C277" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D277">
         <v>10308</v>
@@ -6619,10 +6613,10 @@
         <v>157</v>
       </c>
       <c r="B278" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C278" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="D278">
         <v>10308</v>
@@ -6636,10 +6630,10 @@
         <v>157</v>
       </c>
       <c r="B279" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C279" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="D279">
         <v>10308</v>
@@ -6653,10 +6647,10 @@
         <v>157</v>
       </c>
       <c r="B280" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C280" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="D280">
         <v>10308</v>
@@ -6670,10 +6664,10 @@
         <v>157</v>
       </c>
       <c r="B281" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="C281" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="D281">
         <v>10308</v>
@@ -6687,10 +6681,10 @@
         <v>157</v>
       </c>
       <c r="B282" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C282" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="D282">
         <v>10308</v>
@@ -6704,10 +6698,10 @@
         <v>157</v>
       </c>
       <c r="B283" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C283" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="D283">
         <v>10308</v>
@@ -6721,10 +6715,10 @@
         <v>157</v>
       </c>
       <c r="B284" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C284" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="D284">
         <v>10308</v>
@@ -6738,10 +6732,10 @@
         <v>157</v>
       </c>
       <c r="B285" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C285" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="D285">
         <v>10308</v>
@@ -6755,10 +6749,10 @@
         <v>157</v>
       </c>
       <c r="B286" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C286" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="D286">
         <v>10308</v>
@@ -6772,10 +6766,10 @@
         <v>157</v>
       </c>
       <c r="B287" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C287" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="D287">
         <v>10308</v>
@@ -6789,10 +6783,10 @@
         <v>157</v>
       </c>
       <c r="B288" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C288" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D288">
         <v>10308</v>
@@ -6806,10 +6800,10 @@
         <v>157</v>
       </c>
       <c r="B289" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C289" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="D289">
         <v>10308</v>
@@ -6823,10 +6817,10 @@
         <v>157</v>
       </c>
       <c r="B290" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C290" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="D290">
         <v>10308</v>
@@ -6840,10 +6834,10 @@
         <v>157</v>
       </c>
       <c r="B291" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C291" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="D291">
         <v>10308</v>
@@ -6857,10 +6851,10 @@
         <v>157</v>
       </c>
       <c r="B292" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C292" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="D292">
         <v>10308</v>
@@ -6874,10 +6868,10 @@
         <v>157</v>
       </c>
       <c r="B293" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C293" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="D293">
         <v>10308</v>
@@ -6891,10 +6885,10 @@
         <v>157</v>
       </c>
       <c r="B294" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="C294" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="D294">
         <v>10308</v>
@@ -6908,10 +6902,10 @@
         <v>157</v>
       </c>
       <c r="B295" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C295" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D295">
         <v>10308</v>
@@ -6925,10 +6919,10 @@
         <v>157</v>
       </c>
       <c r="B296" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="C296" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="D296">
         <v>10308</v>
@@ -6942,10 +6936,10 @@
         <v>157</v>
       </c>
       <c r="B297" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C297" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="D297">
         <v>10308</v>
@@ -6959,10 +6953,10 @@
         <v>157</v>
       </c>
       <c r="B298" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C298" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="D298">
         <v>10308</v>
@@ -6976,10 +6970,10 @@
         <v>157</v>
       </c>
       <c r="B299" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C299" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="D299">
         <v>10308</v>
@@ -6993,10 +6987,10 @@
         <v>157</v>
       </c>
       <c r="B300" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="C300" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="D300">
         <v>10308</v>
@@ -7010,10 +7004,10 @@
         <v>157</v>
       </c>
       <c r="B301" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C301" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D301">
         <v>10308</v>
@@ -7027,10 +7021,10 @@
         <v>157</v>
       </c>
       <c r="B302" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="C302" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="D302">
         <v>10308</v>
@@ -7044,10 +7038,10 @@
         <v>157</v>
       </c>
       <c r="B303" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C303" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D303">
         <v>10308</v>
@@ -7061,10 +7055,10 @@
         <v>157</v>
       </c>
       <c r="B304" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C304" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="D304">
         <v>10308</v>
@@ -7078,10 +7072,10 @@
         <v>157</v>
       </c>
       <c r="B305" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="C305" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="D305">
         <v>10308</v>
@@ -7095,10 +7089,10 @@
         <v>157</v>
       </c>
       <c r="B306" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C306" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D306">
         <v>10308</v>
@@ -7112,10 +7106,10 @@
         <v>157</v>
       </c>
       <c r="B307" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="C307" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="D307">
         <v>10308</v>
@@ -7129,10 +7123,10 @@
         <v>157</v>
       </c>
       <c r="B308" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C308" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="D308">
         <v>10308</v>
@@ -7146,10 +7140,10 @@
         <v>157</v>
       </c>
       <c r="B309" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C309" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D309">
         <v>10308</v>
@@ -7163,10 +7157,10 @@
         <v>157</v>
       </c>
       <c r="B310" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="C310" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="D310">
         <v>10308</v>
@@ -7180,10 +7174,10 @@
         <v>157</v>
       </c>
       <c r="B311" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C311" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="D311">
         <v>10308</v>
@@ -7197,10 +7191,10 @@
         <v>157</v>
       </c>
       <c r="B312" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C312" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D312">
         <v>10308</v>
@@ -7214,10 +7208,10 @@
         <v>157</v>
       </c>
       <c r="B313" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C313" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="D313">
         <v>10308</v>
@@ -7231,10 +7225,10 @@
         <v>157</v>
       </c>
       <c r="B314" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C314" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="D314">
         <v>10308</v>
@@ -7248,10 +7242,10 @@
         <v>157</v>
       </c>
       <c r="B315" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C315" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D315">
         <v>10308</v>
@@ -7265,10 +7259,10 @@
         <v>157</v>
       </c>
       <c r="B316" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="C316" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D316">
         <v>10308</v>
@@ -7282,10 +7276,10 @@
         <v>157</v>
       </c>
       <c r="B317" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C317" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D317">
         <v>10308</v>
@@ -7299,10 +7293,10 @@
         <v>157</v>
       </c>
       <c r="B318" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="C318" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="D318">
         <v>10308</v>
@@ -7316,10 +7310,10 @@
         <v>157</v>
       </c>
       <c r="B319" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="C319" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D319">
         <v>10308</v>
@@ -7333,10 +7327,10 @@
         <v>157</v>
       </c>
       <c r="B320" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C320" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D320">
         <v>10308</v>
@@ -7350,10 +7344,10 @@
         <v>157</v>
       </c>
       <c r="B321" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="C321" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="D321">
         <v>10308</v>
@@ -7367,10 +7361,10 @@
         <v>157</v>
       </c>
       <c r="B322" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="C322" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="D322">
         <v>10308</v>
@@ -7384,10 +7378,10 @@
         <v>157</v>
       </c>
       <c r="B323" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C323" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D323">
         <v>10308</v>
@@ -7401,10 +7395,10 @@
         <v>157</v>
       </c>
       <c r="B324" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="C324" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="D324">
         <v>10308</v>
@@ -7418,10 +7412,10 @@
         <v>157</v>
       </c>
       <c r="B325" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C325" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D325">
         <v>10308</v>
@@ -7435,10 +7429,10 @@
         <v>157</v>
       </c>
       <c r="B326" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="C326" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="D326">
         <v>10308</v>
@@ -7452,10 +7446,10 @@
         <v>157</v>
       </c>
       <c r="B327" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="C327" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D327">
         <v>10308</v>
@@ -7469,10 +7463,10 @@
         <v>157</v>
       </c>
       <c r="B328" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C328" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D328">
         <v>10308</v>
@@ -7486,10 +7480,10 @@
         <v>157</v>
       </c>
       <c r="B329" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="C329" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D329">
         <v>10308</v>
@@ -7503,10 +7497,10 @@
         <v>157</v>
       </c>
       <c r="B330" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="C330" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D330">
         <v>10308</v>
@@ -7520,10 +7514,10 @@
         <v>157</v>
       </c>
       <c r="B331" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="C331" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="D331">
         <v>10308</v>
@@ -7537,10 +7531,10 @@
         <v>157</v>
       </c>
       <c r="B332" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="C332" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D332">
         <v>10308</v>
@@ -7554,10 +7548,10 @@
         <v>157</v>
       </c>
       <c r="B333" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="C333" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D333">
         <v>10308</v>
@@ -7571,10 +7565,10 @@
         <v>157</v>
       </c>
       <c r="B334" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="C334" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D334">
         <v>10308</v>
@@ -7588,10 +7582,10 @@
         <v>157</v>
       </c>
       <c r="B335" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="C335" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="D335">
         <v>10308</v>
@@ -7605,10 +7599,10 @@
         <v>157</v>
       </c>
       <c r="B336" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="C336" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D336">
         <v>10308</v>
@@ -7622,10 +7616,10 @@
         <v>157</v>
       </c>
       <c r="B337" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="C337" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D337">
         <v>10308</v>
@@ -7639,10 +7633,10 @@
         <v>157</v>
       </c>
       <c r="B338" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="C338" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D338">
         <v>10308</v>
@@ -7656,10 +7650,10 @@
         <v>157</v>
       </c>
       <c r="B339" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="C339" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
       <c r="D339">
         <v>10308</v>
@@ -7673,10 +7667,10 @@
         <v>157</v>
       </c>
       <c r="B340" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="C340" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D340">
         <v>10308</v>
@@ -7690,10 +7684,10 @@
         <v>157</v>
       </c>
       <c r="B341" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="C341" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="D341">
         <v>10308</v>
@@ -7707,10 +7701,10 @@
         <v>157</v>
       </c>
       <c r="B342" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="C342" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D342">
         <v>10308</v>
@@ -7724,10 +7718,10 @@
         <v>157</v>
       </c>
       <c r="B343" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="C343" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D343">
         <v>10308</v>
@@ -7741,10 +7735,10 @@
         <v>157</v>
       </c>
       <c r="B344" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C344" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D344">
         <v>10308</v>
@@ -7758,10 +7752,10 @@
         <v>157</v>
       </c>
       <c r="B345" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="C345" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D345">
         <v>10308</v>
@@ -7775,16 +7769,16 @@
         <v>157</v>
       </c>
       <c r="B346" t="s">
-        <v>494</v>
+        <v>222</v>
       </c>
       <c r="C346" t="s">
-        <v>495</v>
+        <v>223</v>
       </c>
       <c r="D346">
-        <v>10308</v>
+        <v>10107</v>
       </c>
       <c r="E346" s="3">
-        <v>10309</v>
+        <v>10315</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.35">
@@ -7792,16 +7786,16 @@
         <v>157</v>
       </c>
       <c r="B347" t="s">
-        <v>222</v>
+        <v>158</v>
       </c>
       <c r="C347" t="s">
-        <v>223</v>
+        <v>159</v>
       </c>
       <c r="D347">
-        <v>10107</v>
+        <v>10402</v>
       </c>
       <c r="E347" s="3">
-        <v>10315</v>
+        <v>10311</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.35">
@@ -7809,16 +7803,16 @@
         <v>157</v>
       </c>
       <c r="B348" t="s">
-        <v>158</v>
+        <v>200</v>
       </c>
       <c r="C348" t="s">
-        <v>159</v>
+        <v>201</v>
       </c>
       <c r="D348">
-        <v>10402</v>
+        <v>115</v>
       </c>
       <c r="E348" s="3">
-        <v>10311</v>
+        <v>10609</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.35">
@@ -7826,10 +7820,10 @@
         <v>157</v>
       </c>
       <c r="B349" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C349" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D349">
         <v>115</v>
@@ -7843,10 +7837,10 @@
         <v>157</v>
       </c>
       <c r="B350" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C350" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D350">
         <v>115</v>
@@ -7860,16 +7854,16 @@
         <v>157</v>
       </c>
       <c r="B351" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="C351" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="D351">
+        <v>104</v>
+      </c>
+      <c r="E351" s="3">
         <v>115</v>
-      </c>
-      <c r="E351" s="3">
-        <v>10609</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.35">
@@ -7877,10 +7871,10 @@
         <v>157</v>
       </c>
       <c r="B352" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C352" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D352">
         <v>104</v>
@@ -7894,16 +7888,16 @@
         <v>157</v>
       </c>
       <c r="B353" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C353" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D353">
+        <v>115</v>
+      </c>
+      <c r="E353" s="3">
         <v>104</v>
-      </c>
-      <c r="E353" s="3">
-        <v>115</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.35">
@@ -7911,10 +7905,10 @@
         <v>157</v>
       </c>
       <c r="B354" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="C354" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D354">
         <v>115</v>
@@ -7928,10 +7922,10 @@
         <v>157</v>
       </c>
       <c r="B355" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C355" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D355">
         <v>115</v>
@@ -7945,10 +7939,10 @@
         <v>157</v>
       </c>
       <c r="B356" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="C356" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D356">
         <v>115</v>
@@ -7962,10 +7956,10 @@
         <v>157</v>
       </c>
       <c r="B357" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C357" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D357">
         <v>115</v>
@@ -7979,10 +7973,10 @@
         <v>157</v>
       </c>
       <c r="B358" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C358" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D358">
         <v>115</v>
@@ -7996,10 +7990,10 @@
         <v>157</v>
       </c>
       <c r="B359" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C359" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D359">
         <v>115</v>
@@ -8013,10 +8007,10 @@
         <v>157</v>
       </c>
       <c r="B360" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C360" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D360">
         <v>115</v>
@@ -8026,25 +8020,25 @@
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A361" t="s">
-        <v>157</v>
+      <c r="A361" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B361" t="s">
-        <v>186</v>
+        <v>96</v>
       </c>
       <c r="C361" t="s">
-        <v>187</v>
+        <v>97</v>
       </c>
       <c r="D361">
-        <v>115</v>
+        <v>11615</v>
       </c>
       <c r="E361" s="3">
-        <v>104</v>
+        <v>11601</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A362" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B362" t="s">
         <v>96</v>
@@ -8061,7 +8055,7 @@
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A363" s="1" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="B363" t="s">
         <v>96</v>
@@ -8073,23 +8067,6 @@
         <v>11615</v>
       </c>
       <c r="E363" s="3">
-        <v>11601</v>
-      </c>
-    </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A364" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B364" t="s">
-        <v>96</v>
-      </c>
-      <c r="C364" t="s">
-        <v>97</v>
-      </c>
-      <c r="D364">
-        <v>11615</v>
-      </c>
-      <c r="E364" s="3">
         <v>11601</v>
       </c>
     </row>
@@ -8099,7 +8076,7 @@
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E143">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E142">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>